<commit_message>
updated driver manager functionality
</commit_message>
<xml_diff>
--- a/src/test/resources/data/TestDataSheet.xlsx
+++ b/src/test/resources/data/TestDataSheet.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="155">
   <si>
     <t>password</t>
   </si>
@@ -107,9 +107,6 @@
     <t>Run Mode</t>
   </si>
   <si>
-    <t>Results</t>
-  </si>
-  <si>
     <t>TC001_LoginTest</t>
   </si>
   <si>
@@ -479,16 +476,16 @@
     <t>PASS</t>
   </si>
   <si>
+    <t>Object</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
     <t>FAIL</t>
-  </si>
-  <si>
-    <t>Object</t>
-  </si>
-  <si>
-    <t>Data</t>
-  </si>
-  <si>
-    <t/>
   </si>
 </sst>
 </file>
@@ -902,7 +899,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -925,105 +922,105 @@
         <v>27</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>28</v>
+        <v>150</v>
       </c>
     </row>
     <row customFormat="1" r="2" s="1" spans="1:4">
       <c r="A2" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="D2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>65</v>
-      </c>
       <c r="C4" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D4" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D5" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>110</v>
-      </c>
       <c r="C8" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -1045,7 +1042,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1056,9 +1053,7 @@
     <col min="4" max="4" customWidth="true" style="5" width="21.5703125" collapsed="true"/>
     <col min="5" max="5" customWidth="true" style="5" width="18.5703125" collapsed="true"/>
     <col min="6" max="6" customWidth="true" style="1" width="34.0" collapsed="true"/>
-    <col min="7" max="7" style="5" width="9.140625" collapsed="true"/>
-    <col min="8" max="8" style="5" width="9.140625" collapsed="false"/>
-    <col min="9" max="16384" style="5" width="9.140625" collapsed="true"/>
+    <col min="7" max="16384" style="5" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row customFormat="1" r="1" s="8" spans="1:6">
@@ -1072,13 +1067,13 @@
         <v>22</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>23</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row customFormat="1" r="2" s="1" spans="1:6">
@@ -1086,7 +1081,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>8</v>
@@ -1103,7 +1098,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>14</v>
@@ -1123,7 +1118,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>14</v>
@@ -1143,7 +1138,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>8</v>
@@ -1160,10 +1155,10 @@
         <v>7</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>17</v>
@@ -1200,9 +1195,7 @@
     <col min="4" max="4" bestFit="true" customWidth="true" style="5" width="33.5703125" collapsed="true"/>
     <col min="5" max="5" customWidth="true" style="5" width="18.5703125" collapsed="true"/>
     <col min="6" max="6" customWidth="true" style="1" width="34.0" collapsed="true"/>
-    <col min="7" max="7" style="5" width="9.140625" collapsed="true"/>
-    <col min="8" max="8" style="5" width="9.140625" collapsed="false"/>
-    <col min="9" max="16384" style="5" width="9.140625" collapsed="true"/>
+    <col min="7" max="16384" style="5" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row customFormat="1" r="1" s="8" spans="1:6">
@@ -1216,13 +1209,13 @@
         <v>22</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>23</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row customFormat="1" r="2" s="1" spans="1:6">
@@ -1230,7 +1223,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>8</v>
@@ -1282,7 +1275,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>8</v>
@@ -1299,7 +1292,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>17</v>
@@ -1316,13 +1309,13 @@
         <v>15</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>10</v>
@@ -1333,13 +1326,13 @@
         <v>16</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>10</v>
@@ -1350,10 +1343,10 @@
         <v>18</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>10</v>
@@ -1361,13 +1354,13 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C10" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>56</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>57</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>10</v>
@@ -1375,16 +1368,16 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>10</v>
@@ -1392,21 +1385,21 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>10</v>
@@ -1414,27 +1407,27 @@
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>19</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>10</v>
@@ -1442,16 +1435,16 @@
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>10</v>
@@ -1459,33 +1452,33 @@
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>10</v>
@@ -1493,33 +1486,33 @@
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>10</v>
@@ -1527,16 +1520,16 @@
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>10</v>
@@ -1544,13 +1537,13 @@
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>17</v>
@@ -1559,7 +1552,7 @@
         <v>10</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1587,8 +1580,7 @@
     <col min="4" max="4" customWidth="true" style="5" width="21.5703125" collapsed="true"/>
     <col min="5" max="5" customWidth="true" style="5" width="18.5703125" collapsed="true"/>
     <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="37.42578125" collapsed="true"/>
-    <col min="7" max="7" style="5" width="9.140625" collapsed="false"/>
-    <col min="8" max="16384" style="5" width="9.140625" collapsed="true"/>
+    <col min="7" max="16384" style="5" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row customFormat="1" r="1" s="8" spans="1:6">
@@ -1602,13 +1594,13 @@
         <v>22</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>23</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row customFormat="1" r="2" s="1" spans="1:6">
@@ -1616,7 +1608,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>8</v>
@@ -1633,13 +1625,13 @@
         <v>4</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>67</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>12</v>
@@ -1651,13 +1643,13 @@
         <v>5</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>12</v>
@@ -1668,10 +1660,10 @@
         <v>6</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>10</v>
@@ -1682,7 +1674,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>17</v>
@@ -1691,7 +1683,7 @@
         <v>10</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1702,7 +1694,7 @@
         <v>8</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>10</v>
@@ -1716,13 +1708,13 @@
         <v>14</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>12</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -1733,18 +1725,18 @@
         <v>14</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>12</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>14</v>
@@ -1761,121 +1753,121 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>12</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>12</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C13" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D14" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>12</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D16" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>12</v>
@@ -1883,13 +1875,13 @@
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>17</v>
@@ -1912,7 +1904,7 @@
   <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1923,8 +1915,7 @@
     <col min="4" max="4" customWidth="true" style="5" width="21.5703125" collapsed="true"/>
     <col min="5" max="5" customWidth="true" style="5" width="18.5703125" collapsed="true"/>
     <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="37.42578125" collapsed="true"/>
-    <col min="7" max="7" style="5" width="9.140625" collapsed="false"/>
-    <col min="8" max="16384" style="5" width="9.140625" collapsed="true"/>
+    <col min="7" max="16384" style="5" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row customFormat="1" r="1" s="8" spans="1:6">
@@ -1938,13 +1929,13 @@
         <v>22</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>23</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row customFormat="1" r="2" s="1" spans="1:6">
@@ -1952,7 +1943,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>8</v>
@@ -1969,13 +1960,13 @@
         <v>4</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>67</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>12</v>
@@ -1987,13 +1978,13 @@
         <v>5</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>12</v>
@@ -2004,10 +1995,10 @@
         <v>6</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>10</v>
@@ -2018,7 +2009,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>17</v>
@@ -2027,7 +2018,7 @@
         <v>10</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -2038,7 +2029,7 @@
         <v>8</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>10</v>
@@ -2052,13 +2043,13 @@
         <v>14</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>12</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -2069,18 +2060,18 @@
         <v>14</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>12</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>14</v>
@@ -2097,121 +2088,121 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>12</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>12</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C13" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D14" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>12</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D16" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>12</v>
@@ -2219,13 +2210,13 @@
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>17</v>
@@ -2239,16 +2230,16 @@
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>10</v>
@@ -2256,16 +2247,16 @@
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>10</v>
@@ -2273,13 +2264,13 @@
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>10</v>
@@ -2287,13 +2278,13 @@
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C22" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D22" s="5" t="s">
         <v>56</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>57</v>
       </c>
       <c r="E22" s="5" t="s">
         <v>10</v>
@@ -2301,16 +2292,16 @@
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>10</v>
@@ -2318,21 +2309,21 @@
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E25" s="5" t="s">
         <v>10</v>
@@ -2346,21 +2337,21 @@
         <v>19</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E27" s="5" t="s">
         <v>10</v>
@@ -2368,16 +2359,16 @@
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E28" s="5" t="s">
         <v>10</v>
@@ -2385,33 +2376,33 @@
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E30" s="5" t="s">
         <v>10</v>
@@ -2419,33 +2410,33 @@
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E32" s="5" t="s">
         <v>10</v>
@@ -2453,16 +2444,16 @@
     </row>
     <row r="33" spans="1:6">
       <c r="A33" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C33" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E33" s="5" t="s">
         <v>10</v>
@@ -2470,13 +2461,13 @@
     </row>
     <row r="34" spans="1:6">
       <c r="A34" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D34" s="5" t="s">
         <v>17</v>
@@ -2485,7 +2476,7 @@
         <v>10</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -2510,8 +2501,7 @@
     <col min="4" max="4" customWidth="true" style="5" width="21.5703125" collapsed="true"/>
     <col min="5" max="5" customWidth="true" style="5" width="18.5703125" collapsed="true"/>
     <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="37.42578125" collapsed="true"/>
-    <col min="7" max="7" style="5" width="9.140625" collapsed="false"/>
-    <col min="8" max="16384" style="5" width="9.140625" collapsed="true"/>
+    <col min="7" max="16384" style="5" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row customFormat="1" r="1" s="8" spans="1:6">
@@ -2525,13 +2515,13 @@
         <v>22</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>23</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -2539,13 +2529,13 @@
         <v>3</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>10</v>
@@ -2556,10 +2546,10 @@
         <v>4</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>10</v>
@@ -2570,10 +2560,10 @@
         <v>5</v>
       </c>
       <c r="C4" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>56</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>57</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>10</v>
@@ -2584,13 +2574,13 @@
         <v>6</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>10</v>
@@ -2601,7 +2591,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -2609,10 +2599,10 @@
         <v>15</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>10</v>
@@ -2626,7 +2616,7 @@
         <v>19</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -2634,13 +2624,13 @@
         <v>18</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>10</v>
@@ -2648,13 +2638,13 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>10</v>
@@ -2662,7 +2652,7 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>14</v>
@@ -2679,10 +2669,10 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>14</v>
@@ -2699,10 +2689,10 @@
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>8</v>
@@ -2716,33 +2706,33 @@
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>10</v>
@@ -2750,33 +2740,33 @@
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>10</v>
@@ -2784,16 +2774,16 @@
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>10</v>
@@ -2801,13 +2791,13 @@
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>17</v>
@@ -2816,7 +2806,7 @@
         <v>10</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -2844,8 +2834,7 @@
     <col min="4" max="4" customWidth="true" style="5" width="21.5703125" collapsed="true"/>
     <col min="5" max="5" customWidth="true" style="5" width="18.5703125" collapsed="true"/>
     <col min="6" max="6" customWidth="true" style="1" width="17.28515625" collapsed="true"/>
-    <col min="7" max="7" style="5" width="9.140625" collapsed="false"/>
-    <col min="8" max="16384" style="5" width="9.140625" collapsed="true"/>
+    <col min="7" max="16384" style="5" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row customFormat="1" r="1" s="8" spans="1:6">
@@ -2859,13 +2848,13 @@
         <v>22</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>23</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -2873,19 +2862,19 @@
         <v>3</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -2893,16 +2882,16 @@
         <v>4</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -2910,16 +2899,16 @@
         <v>5</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>10</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -2927,19 +2916,19 @@
         <v>6</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C5" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>116</v>
-      </c>
       <c r="E5" s="5" t="s">
         <v>10</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -2947,13 +2936,13 @@
         <v>7</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C6" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>117</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>118</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>10</v>
@@ -2980,8 +2969,7 @@
     <col min="4" max="4" customWidth="true" style="5" width="21.5703125" collapsed="true"/>
     <col min="5" max="5" customWidth="true" style="5" width="18.5703125" collapsed="true"/>
     <col min="6" max="6" customWidth="true" style="1" width="20.7109375" collapsed="true"/>
-    <col min="7" max="7" style="5" width="9.140625" collapsed="false"/>
-    <col min="8" max="16384" style="5" width="9.140625" collapsed="true"/>
+    <col min="7" max="16384" style="5" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row customFormat="1" r="1" s="8" spans="1:6">
@@ -2995,13 +2983,13 @@
         <v>22</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>23</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -3009,19 +2997,19 @@
         <v>3</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -3029,16 +3017,16 @@
         <v>4</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -3046,16 +3034,16 @@
         <v>5</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>10</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -3063,19 +3051,19 @@
         <v>6</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C5" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>116</v>
-      </c>
       <c r="E5" s="5" t="s">
         <v>10</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -3083,13 +3071,13 @@
         <v>7</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C6" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>117</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>118</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
Updated code for parallel run
</commit_message>
<xml_diff>
--- a/src/test/resources/data/TestDataSheet.xlsx
+++ b/src/test/resources/data/TestDataSheet.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="155">
   <si>
     <t>password</t>
   </si>
@@ -359,130 +359,130 @@
     <t>searchButton</t>
   </si>
   <si>
+    <t>searchResultHeading</t>
+  </si>
+  <si>
+    <t>validateSearchResults</t>
+  </si>
+  <si>
+    <t>searchResults</t>
+  </si>
+  <si>
+    <t>validateSearchResultCount</t>
+  </si>
+  <si>
+    <t>searchResultCount</t>
+  </si>
+  <si>
+    <t>Blouse</t>
+  </si>
+  <si>
+    <t>Clicking on Sign in Link</t>
+  </si>
+  <si>
+    <t>Enter email ID</t>
+  </si>
+  <si>
+    <t>Enter password</t>
+  </si>
+  <si>
+    <t>Clicking on Login Button</t>
+  </si>
+  <si>
+    <t>Validating the page heading</t>
+  </si>
+  <si>
+    <t>Click on Add To Cart Button</t>
+  </si>
+  <si>
+    <t>Procced to Order Summary</t>
+  </si>
+  <si>
+    <t>Procced to Address Details</t>
+  </si>
+  <si>
+    <t>Procced to Shipping Details</t>
+  </si>
+  <si>
+    <t>Accept Terms &amp; Conditions</t>
+  </si>
+  <si>
+    <t>Procced to Payment</t>
+  </si>
+  <si>
+    <t>Select Pay by Cheque option</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Confirm the Order </t>
+  </si>
+  <si>
+    <t>Verify that Order is confirmed</t>
+  </si>
+  <si>
+    <t>Select Women category to choose a product</t>
+  </si>
+  <si>
+    <t>Clicking on one of the Product</t>
+  </si>
+  <si>
+    <t>Enter Login Credentials to log in</t>
+  </si>
+  <si>
+    <t>Enter a unique email ID to create new Account</t>
+  </si>
+  <si>
+    <t>Click on Create Accont button to create new Account</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enter Detials in all the madatory fields to create an Account </t>
+  </si>
+  <si>
+    <t>Click on Register button</t>
+  </si>
+  <si>
+    <t>Vierify that New Account is created and logged in</t>
+  </si>
+  <si>
+    <t>Enter valid login credentials</t>
+  </si>
+  <si>
+    <t>Search for the product</t>
+  </si>
+  <si>
+    <t>Verify that search result is same as the product searched</t>
+  </si>
+  <si>
+    <t>Verify that search result count is same as the product displayed on the screen.</t>
+  </si>
+  <si>
+    <t>Enter complete prodct name</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>validateDataOnScreenMatches</t>
+  </si>
+  <si>
+    <t>validateDataOnScreenContains</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t>Object</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
     <t>Printed</t>
   </si>
   <si>
-    <t>searchResultHeading</t>
-  </si>
-  <si>
-    <t>validateSearchResults</t>
-  </si>
-  <si>
-    <t>searchResults</t>
-  </si>
-  <si>
-    <t>validateSearchResultCount</t>
-  </si>
-  <si>
-    <t>searchResultCount</t>
-  </si>
-  <si>
-    <t>Blouse</t>
-  </si>
-  <si>
-    <t>Clicking on Sign in Link</t>
-  </si>
-  <si>
-    <t>Enter email ID</t>
-  </si>
-  <si>
-    <t>Enter password</t>
-  </si>
-  <si>
-    <t>Clicking on Login Button</t>
-  </si>
-  <si>
-    <t>Validating the page heading</t>
-  </si>
-  <si>
-    <t>Click on Add To Cart Button</t>
-  </si>
-  <si>
-    <t>Procced to Order Summary</t>
-  </si>
-  <si>
-    <t>Procced to Address Details</t>
-  </si>
-  <si>
-    <t>Procced to Shipping Details</t>
-  </si>
-  <si>
-    <t>Accept Terms &amp; Conditions</t>
-  </si>
-  <si>
-    <t>Procced to Payment</t>
-  </si>
-  <si>
-    <t>Select Pay by Cheque option</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Confirm the Order </t>
-  </si>
-  <si>
-    <t>Verify that Order is confirmed</t>
-  </si>
-  <si>
-    <t>Select Women category to choose a product</t>
-  </si>
-  <si>
-    <t>Clicking on one of the Product</t>
-  </si>
-  <si>
-    <t>Enter Login Credentials to log in</t>
-  </si>
-  <si>
-    <t>Enter a unique email ID to create new Account</t>
-  </si>
-  <si>
-    <t>Click on Create Accont button to create new Account</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Enter Detials in all the madatory fields to create an Account </t>
-  </si>
-  <si>
-    <t>Click on Register button</t>
-  </si>
-  <si>
-    <t>Vierify that New Account is created and logged in</t>
-  </si>
-  <si>
-    <t>Enter valid login credentials</t>
-  </si>
-  <si>
     <t>Enter partial prodct name</t>
-  </si>
-  <si>
-    <t>Search for the product</t>
-  </si>
-  <si>
-    <t>Verify that search result is same as the product searched</t>
-  </si>
-  <si>
-    <t>Verify that search result count is same as the product displayed on the screen.</t>
-  </si>
-  <si>
-    <t>Enter complete prodct name</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>validateDataOnScreenMatches</t>
-  </si>
-  <si>
-    <t>validateDataOnScreenContains</t>
-  </si>
-  <si>
-    <t>PASS</t>
-  </si>
-  <si>
-    <t>Object</t>
-  </si>
-  <si>
-    <t>Data</t>
-  </si>
-  <si>
-    <t/>
   </si>
   <si>
     <t>FAIL</t>
@@ -899,7 +899,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -922,7 +922,7 @@
         <v>27</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row customFormat="1" r="2" s="1" spans="1:4">
@@ -936,7 +936,7 @@
         <v>30</v>
       </c>
       <c r="D2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -950,7 +950,7 @@
         <v>30</v>
       </c>
       <c r="D3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -964,7 +964,7 @@
         <v>30</v>
       </c>
       <c r="D4" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -978,7 +978,7 @@
         <v>30</v>
       </c>
       <c r="D5" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -992,7 +992,7 @@
         <v>30</v>
       </c>
       <c r="D6" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -1006,7 +1006,7 @@
         <v>30</v>
       </c>
       <c r="D7" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -1020,7 +1020,7 @@
         <v>30</v>
       </c>
       <c r="D8" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -1041,9 +1041,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -1067,13 +1065,13 @@
         <v>22</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>23</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row customFormat="1" r="2" s="1" spans="1:6">
@@ -1081,7 +1079,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>8</v>
@@ -1098,7 +1096,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>14</v>
@@ -1118,7 +1116,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>14</v>
@@ -1138,7 +1136,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>8</v>
@@ -1155,10 +1153,10 @@
         <v>7</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>17</v>
@@ -1184,7 +1182,7 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1209,13 +1207,13 @@
         <v>22</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>23</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row customFormat="1" r="2" s="1" spans="1:6">
@@ -1223,7 +1221,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>8</v>
@@ -1275,7 +1273,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>8</v>
@@ -1292,7 +1290,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>17</v>
@@ -1309,7 +1307,7 @@
         <v>15</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>8</v>
@@ -1326,7 +1324,7 @@
         <v>16</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>61</v>
@@ -1371,7 +1369,7 @@
         <v>44</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>8</v>
@@ -1421,7 +1419,7 @@
         <v>48</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>61</v>
@@ -1438,7 +1436,7 @@
         <v>49</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>8</v>
@@ -1455,7 +1453,7 @@
         <v>50</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>8</v>
@@ -1472,7 +1470,7 @@
         <v>57</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>8</v>
@@ -1489,7 +1487,7 @@
         <v>58</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>8</v>
@@ -1506,7 +1504,7 @@
         <v>59</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>8</v>
@@ -1523,7 +1521,7 @@
         <v>62</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>8</v>
@@ -1540,10 +1538,10 @@
         <v>91</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>17</v>
@@ -1569,7 +1567,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1594,13 +1592,13 @@
         <v>22</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>23</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row customFormat="1" r="2" s="1" spans="1:6">
@@ -1608,7 +1606,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>8</v>
@@ -1625,7 +1623,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>65</v>
@@ -1643,7 +1641,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>8</v>
@@ -1674,7 +1672,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>17</v>
@@ -1841,7 +1839,7 @@
         <v>49</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>87</v>
@@ -1861,7 +1859,7 @@
         <v>50</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>8</v>
@@ -1878,10 +1876,10 @@
         <v>57</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>17</v>
@@ -1904,7 +1902,7 @@
   <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1929,13 +1927,13 @@
         <v>22</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>23</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row customFormat="1" r="2" s="1" spans="1:6">
@@ -1943,7 +1941,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>8</v>
@@ -1960,7 +1958,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>65</v>
@@ -1978,7 +1976,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>8</v>
@@ -2009,7 +2007,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>17</v>
@@ -2176,7 +2174,7 @@
         <v>49</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>87</v>
@@ -2196,7 +2194,7 @@
         <v>50</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>8</v>
@@ -2213,10 +2211,10 @@
         <v>57</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>17</v>
@@ -2233,7 +2231,7 @@
         <v>58</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>8</v>
@@ -2250,7 +2248,7 @@
         <v>59</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>61</v>
@@ -2295,7 +2293,7 @@
         <v>92</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>8</v>
@@ -2337,7 +2335,7 @@
         <v>19</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -2345,7 +2343,7 @@
         <v>95</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>61</v>
@@ -2362,7 +2360,7 @@
         <v>96</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>8</v>
@@ -2379,7 +2377,7 @@
         <v>97</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>8</v>
@@ -2396,7 +2394,7 @@
         <v>98</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>8</v>
@@ -2413,7 +2411,7 @@
         <v>99</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>8</v>
@@ -2430,7 +2428,7 @@
         <v>100</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>8</v>
@@ -2447,7 +2445,7 @@
         <v>101</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C33" s="5" t="s">
         <v>8</v>
@@ -2464,10 +2462,10 @@
         <v>102</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D34" s="5" t="s">
         <v>17</v>
@@ -2490,7 +2488,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2515,13 +2513,13 @@
         <v>22</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>23</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -2529,7 +2527,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>8</v>
@@ -2574,7 +2572,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>8</v>
@@ -2593,6 +2591,7 @@
       <c r="C6" s="5" t="s">
         <v>60</v>
       </c>
+      <c r="D6"/>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="1" t="s">
@@ -2624,7 +2623,7 @@
         <v>18</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>61</v>
@@ -2672,7 +2671,7 @@
         <v>45</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>14</v>
@@ -2692,7 +2691,7 @@
         <v>46</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>8</v>
@@ -2709,7 +2708,7 @@
         <v>47</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>8</v>
@@ -2726,7 +2725,7 @@
         <v>48</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>8</v>
@@ -2743,7 +2742,7 @@
         <v>49</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>8</v>
@@ -2760,7 +2759,7 @@
         <v>50</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>8</v>
@@ -2777,7 +2776,7 @@
         <v>57</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>8</v>
@@ -2794,10 +2793,10 @@
         <v>58</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>17</v>
@@ -2823,142 +2822,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="5" width="6.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="5" width="71.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="5" width="29.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="5" width="21.5703125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="5" width="18.5703125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="1" width="17.28515625" collapsed="true"/>
-    <col min="7" max="16384" style="5" width="9.140625" collapsed="true"/>
-  </cols>
-  <sheetData>
-    <row customFormat="1" r="1" s="8" spans="1:6">
-      <c r="A1" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2983,13 +2847,13 @@
         <v>22</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>23</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -2997,7 +2861,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>14</v>
@@ -3009,7 +2873,7 @@
         <v>12</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>118</v>
+        <v>152</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -3017,7 +2881,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>8</v>
@@ -3034,16 +2898,16 @@
         <v>5</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>10</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>118</v>
+        <v>152</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -3051,19 +2915,19 @@
         <v>6</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C5" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>115</v>
-      </c>
       <c r="E5" s="5" t="s">
         <v>10</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>118</v>
+        <v>152</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -3071,13 +2935,148 @@
         <v>7</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C6" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>116</v>
       </c>
+      <c r="E6" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="5" width="6.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="5" width="71.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="5" width="29.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="5" width="21.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="5" width="18.5703125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="20.7109375" collapsed="true"/>
+    <col min="7" max="16384" style="5" width="9.140625" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row customFormat="1" r="1" s="8" spans="1:6">
+      <c r="A1" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>115</v>
+      </c>
       <c r="D6" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
Updated excel reader handle parallel run
</commit_message>
<xml_diff>
--- a/src/test/resources/data/TestDataSheet.xlsx
+++ b/src/test/resources/data/TestDataSheet.xlsx
@@ -4,24 +4,24 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView windowHeight="3240" windowWidth="14835" xWindow="0" yWindow="2520"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="14835" windowHeight="3240"/>
   </bookViews>
   <sheets>
-    <sheet name="TestCases" r:id="rId1" sheetId="4"/>
-    <sheet name="TC001_LoginTest" r:id="rId2" sheetId="3"/>
-    <sheet name="TC002_PlaceOrderTest" r:id="rId3" sheetId="2"/>
-    <sheet name="TC003_CreateAccountTest" r:id="rId4" sheetId="5"/>
-    <sheet name="TC004_PlaceOrderWithNewAccount" r:id="rId5" sheetId="6"/>
-    <sheet name="TC005_PlaceOrderAndSignIn" r:id="rId6" sheetId="7"/>
-    <sheet name="TC006_PartialWordSearchTest" r:id="rId7" sheetId="8"/>
-    <sheet name="TC007_CompleteWordSearchTest" r:id="rId8" sheetId="9"/>
+    <sheet name="TestCases" sheetId="4" r:id="rId1"/>
+    <sheet name="TC001_LoginTest" sheetId="3" r:id="rId2"/>
+    <sheet name="TC002_PlaceOrderTest" sheetId="2" r:id="rId3"/>
+    <sheet name="TC003_CreateAccountTest" sheetId="5" r:id="rId4"/>
+    <sheet name="TC004_PlaceOrderWithNewAccount" sheetId="6" r:id="rId5"/>
+    <sheet name="TC005_PlaceOrderAndSignIn" sheetId="7" r:id="rId6"/>
+    <sheet name="TC006_PartialWordSearchTest" sheetId="8" r:id="rId7"/>
+    <sheet name="TC007_CompleteWordSearchTest" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="153">
   <si>
     <t>password</t>
   </si>
@@ -476,23 +476,16 @@
     <t>Data</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>Printed</t>
   </si>
   <si>
     <t>Enter partial prodct name</t>
-  </si>
-  <si>
-    <t>FAIL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -567,47 +560,47 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="11">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="2" fontId="1" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="2" fontId="1" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="2" fontId="1" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
@@ -616,10 +609,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -775,7 +768,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -784,13 +777,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -800,7 +793,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -809,7 +802,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -818,7 +811,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -828,12 +821,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
+            <a:lightRig rig="threePt" dir="t">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT h="25400" w="63500"/>
+            <a:bevelT w="63500" h="25400"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -864,7 +857,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -883,7 +876,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -896,19 +889,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D2" sqref="D2:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="5" width="37.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="5" width="67.5703125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="5" width="10.140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="5" width="15.85546875" collapsed="true"/>
-    <col min="5" max="16384" style="5" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="37.140625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="67.5703125" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.140625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15.85546875" style="5" customWidth="1" collapsed="1"/>
+    <col min="5" max="16384" width="9.140625" style="5" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -925,7 +918,7 @@
         <v>148</v>
       </c>
     </row>
-    <row customFormat="1" r="2" s="1" spans="1:4">
+    <row r="2" spans="1:4" s="1" customFormat="1">
       <c r="A2" s="9" t="s">
         <v>28</v>
       </c>
@@ -935,9 +928,7 @@
       <c r="C2" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D2" t="s">
-        <v>148</v>
-      </c>
+      <c r="D2"/>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="9" t="s">
@@ -949,9 +940,7 @@
       <c r="C3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D3" t="s">
-        <v>148</v>
-      </c>
+      <c r="D3"/>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="10" t="s">
@@ -963,9 +952,7 @@
       <c r="C4" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D4" t="s">
-        <v>148</v>
-      </c>
+      <c r="D4"/>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="9" t="s">
@@ -977,9 +964,7 @@
       <c r="C5" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D5" t="s">
-        <v>148</v>
-      </c>
+      <c r="D5"/>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="10" t="s">
@@ -991,9 +976,7 @@
       <c r="C6" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D6" t="s">
-        <v>148</v>
-      </c>
+      <c r="D6"/>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="10" t="s">
@@ -1005,9 +988,7 @@
       <c r="C7" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D7" t="s">
-        <v>148</v>
-      </c>
+      <c r="D7"/>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="10" t="s">
@@ -1019,42 +1000,40 @@
       <c r="C8" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D8" t="s">
-        <v>148</v>
-      </c>
+      <c r="D8"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink display="TC001_LoginTest" location="TC001_LoginTest!A1" ref="A2"/>
-    <hyperlink display="TC002_PlaceOrderTest" location="TC002_PlaceOrderTest!A1" ref="A3"/>
-    <hyperlink display="TC003_CreateAccountTest" location="TC003_CreateAccountTest!A1" ref="A4"/>
-    <hyperlink display="TC004_PlaceOrderWithNewAccount" location="TC004_PlaceOrderWithNewAccount!A1" ref="A5"/>
-    <hyperlink display="TC005_PlaceOrderAndSignIn" location="TC005_PlaceOrderAndSignIn!A1" ref="A6"/>
-    <hyperlink display="TC006_PartialWordSearchTest" location="TC006_PartialWordSearchTest!A1" ref="A7"/>
-    <hyperlink display="TC007_CompleteWordSearchTest" location="TC007_CompleteWordSearchTest!A1" ref="A8"/>
+    <hyperlink ref="A2" location="TC001_LoginTest!A1" display="TC001_LoginTest"/>
+    <hyperlink ref="A3" location="TC002_PlaceOrderTest!A1" display="TC002_PlaceOrderTest"/>
+    <hyperlink ref="A4" location="TC003_CreateAccountTest!A1" display="TC003_CreateAccountTest"/>
+    <hyperlink ref="A5" location="TC004_PlaceOrderWithNewAccount!A1" display="TC004_PlaceOrderWithNewAccount"/>
+    <hyperlink ref="A6" location="TC005_PlaceOrderAndSignIn!A1" display="TC005_PlaceOrderAndSignIn"/>
+    <hyperlink ref="A7" location="TC006_PartialWordSearchTest!A1" display="TC006_PartialWordSearchTest"/>
+    <hyperlink ref="A8" location="TC007_CompleteWordSearchTest!A1" display="TC007_CompleteWordSearchTest"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="5" width="5.7109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="5" width="53.5703125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="5" width="28.7109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="5" width="21.5703125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="5" width="18.5703125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="1" width="34.0" collapsed="true"/>
-    <col min="7" max="16384" style="5" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="5.7109375" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="53.5703125" style="5" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="28.7109375" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="21.5703125" style="5" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="18.5703125" style="5" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="34" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="16384" width="9.140625" style="5" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="8" spans="1:6">
+    <row r="1" spans="1:6" s="8" customFormat="1">
       <c r="A1" s="6" t="s">
         <v>21</v>
       </c>
@@ -1074,7 +1053,7 @@
         <v>150</v>
       </c>
     </row>
-    <row customFormat="1" r="2" s="1" spans="1:6">
+    <row r="2" spans="1:6" s="1" customFormat="1">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -1091,7 +1070,7 @@
         <v>10</v>
       </c>
     </row>
-    <row customFormat="1" r="3" s="1" spans="1:6">
+    <row r="3" spans="1:6" s="1" customFormat="1">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -1170,16 +1149,16 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="F3"/>
+    <hyperlink ref="F3" r:id="rId1"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="300" orientation="portrait" r:id="rId2" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
@@ -1187,16 +1166,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="5" width="6.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="5" width="53.5703125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="5" width="28.7109375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="5" width="33.5703125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="5" width="18.5703125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="1" width="34.0" collapsed="true"/>
-    <col min="7" max="16384" style="5" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="6" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="53.5703125" style="5" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="28.7109375" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="33.5703125" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="18.5703125" style="5" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="34" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="16384" width="9.140625" style="5" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="8" spans="1:6">
+    <row r="1" spans="1:6" s="8" customFormat="1">
       <c r="A1" s="6" t="s">
         <v>21</v>
       </c>
@@ -1216,7 +1195,7 @@
         <v>150</v>
       </c>
     </row>
-    <row customFormat="1" r="2" s="1" spans="1:6">
+    <row r="2" spans="1:6" s="1" customFormat="1">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -1233,7 +1212,7 @@
         <v>10</v>
       </c>
     </row>
-    <row customFormat="1" r="3" s="1" spans="1:6">
+    <row r="3" spans="1:6" s="1" customFormat="1">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -1555,16 +1534,16 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="F3"/>
+    <hyperlink ref="F3" r:id="rId1"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="300" orientation="portrait" r:id="rId2" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
@@ -1572,16 +1551,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="5" width="5.7109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="5" width="53.5703125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="5" width="28.7109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="5" width="21.5703125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="5" width="18.5703125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="37.42578125" collapsed="true"/>
-    <col min="7" max="16384" style="5" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="5.7109375" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="53.5703125" style="5" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="28.7109375" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="21.5703125" style="5" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="18.5703125" style="5" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="37.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="16384" width="9.140625" style="5" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="8" spans="1:6">
+    <row r="1" spans="1:6" s="8" customFormat="1">
       <c r="A1" s="6" t="s">
         <v>21</v>
       </c>
@@ -1601,7 +1580,7 @@
         <v>150</v>
       </c>
     </row>
-    <row customFormat="1" r="2" s="1" spans="1:6">
+    <row r="2" spans="1:6" s="1" customFormat="1">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -1618,7 +1597,7 @@
         <v>10</v>
       </c>
     </row>
-    <row customFormat="1" r="3" s="1" spans="1:6">
+    <row r="3" spans="1:6" s="1" customFormat="1">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -1892,14 +1871,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="300" orientation="portrait" r:id="rId1" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G34"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
@@ -1907,16 +1886,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="5" width="5.7109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="5" width="53.5703125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="5" width="28.7109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="5" width="21.5703125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="5" width="18.5703125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="37.42578125" collapsed="true"/>
-    <col min="7" max="16384" style="5" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="5.7109375" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="53.5703125" style="5" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="28.7109375" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="21.5703125" style="5" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="18.5703125" style="5" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="37.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="16384" width="9.140625" style="5" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="8" spans="1:6">
+    <row r="1" spans="1:6" s="8" customFormat="1">
       <c r="A1" s="6" t="s">
         <v>21</v>
       </c>
@@ -1936,7 +1915,7 @@
         <v>150</v>
       </c>
     </row>
-    <row customFormat="1" r="2" s="1" spans="1:6">
+    <row r="2" spans="1:6" s="1" customFormat="1">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -1953,7 +1932,7 @@
         <v>10</v>
       </c>
     </row>
-    <row customFormat="1" r="3" s="1" spans="1:6">
+    <row r="3" spans="1:6" s="1" customFormat="1">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -2478,14 +2457,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="300" orientation="portrait" r:id="rId1" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
@@ -2493,16 +2472,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="5" width="6.5703125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="5" width="53.5703125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="5" width="28.7109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="5" width="21.5703125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="5" width="18.5703125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="37.42578125" collapsed="true"/>
-    <col min="7" max="16384" style="5" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="6.5703125" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="53.5703125" style="5" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="28.7109375" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="21.5703125" style="5" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="18.5703125" style="5" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="37.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="16384" width="9.140625" style="5" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="8" spans="1:6">
+    <row r="1" spans="1:6" s="8" customFormat="1">
       <c r="A1" s="6" t="s">
         <v>21</v>
       </c>
@@ -2810,16 +2789,16 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="F11"/>
+    <hyperlink ref="F11" r:id="rId1"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="300" orientation="portrait" r:id="rId2" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
@@ -2827,16 +2806,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="5" width="6.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="5" width="71.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="5" width="29.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="5" width="21.5703125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="5" width="18.5703125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="1" width="20.7109375" collapsed="true"/>
-    <col min="7" max="16384" style="5" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="6.5703125" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="71.7109375" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="29" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="21.5703125" style="5" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="18.5703125" style="5" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="20.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="16384" width="9.140625" style="5" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="8" spans="1:6">
+    <row r="1" spans="1:6" s="8" customFormat="1">
       <c r="A1" s="6" t="s">
         <v>21</v>
       </c>
@@ -2861,7 +2840,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>14</v>
@@ -2873,7 +2852,7 @@
         <v>12</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -2907,7 +2886,7 @@
         <v>10</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -2927,7 +2906,7 @@
         <v>10</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -2948,13 +2927,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
@@ -2962,16 +2941,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="5" width="6.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="5" width="71.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="5" width="29.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="5" width="21.5703125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="5" width="18.5703125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="1" width="20.7109375" collapsed="true"/>
-    <col min="7" max="16384" style="5" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="6.5703125" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="71.7109375" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="29" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="21.5703125" style="5" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="18.5703125" style="5" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="20.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="16384" width="9.140625" style="5" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="8" spans="1:6">
+    <row r="1" spans="1:6" s="8" customFormat="1">
       <c r="A1" s="6" t="s">
         <v>21</v>
       </c>
@@ -3083,6 +3062,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added cart remove test
</commit_message>
<xml_diff>
--- a/src/test/resources/data/TestDataSheet.xlsx
+++ b/src/test/resources/data/TestDataSheet.xlsx
@@ -8,12 +8,12 @@
   </bookViews>
   <sheets>
     <sheet name="TestCases" r:id="rId1" sheetId="4"/>
-    <sheet name="TC001_LoginTest" r:id="rId2" sheetId="3"/>
-    <sheet name="TC002_PlaceOrderTest" r:id="rId3" sheetId="2"/>
-    <sheet name="TC003_CreateAccountTest" r:id="rId4" sheetId="5"/>
+    <sheet name="TC001_RemovePetFromCart" r:id="rId2" sheetId="3"/>
+    <sheet name="TC002_PlaceOrder" r:id="rId3" sheetId="2"/>
+    <sheet name="TC003_CreateAccount" r:id="rId4" sheetId="5"/>
     <sheet name="TC004_PlaceOrderWithNewAccount" r:id="rId5" sheetId="6"/>
     <sheet name="TC005_PlaceOrderAndSignIn" r:id="rId6" sheetId="7"/>
-    <sheet name="TC006_PartialWordSearchTest" r:id="rId7" sheetId="8"/>
+    <sheet name="TC006_DeleteOrder" r:id="rId7" sheetId="8"/>
     <sheet name="TC007_CompleteWordSearchTest" r:id="rId8" sheetId="9"/>
   </sheets>
   <calcPr calcId="125725"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="124">
   <si>
     <t>TS_01</t>
   </si>
@@ -80,12 +80,6 @@
     <t>Run Mode</t>
   </si>
   <si>
-    <t>TC001_LoginTest</t>
-  </si>
-  <si>
-    <t>To verify that user is able to log into the application successfully</t>
-  </si>
-  <si>
     <t>Yes</t>
   </si>
   <si>
@@ -116,12 +110,6 @@
     <t>TS_14</t>
   </si>
   <si>
-    <t>TC002_PlaceOrderTest</t>
-  </si>
-  <si>
-    <t>TC003_CreateAccountTest</t>
-  </si>
-  <si>
     <t>To verify that user is able to create an account successfully</t>
   </si>
   <si>
@@ -137,15 +125,6 @@
     <t>To verify that user is able to place an order successfully as registered user</t>
   </si>
   <si>
-    <t>To select a product and signin while placing the order</t>
-  </si>
-  <si>
-    <t>To validate search result with partial word search</t>
-  </si>
-  <si>
-    <t>TC006_PartialWordSearchTest</t>
-  </si>
-  <si>
     <t>TC007_CompleteWordSearchTest</t>
   </si>
   <si>
@@ -200,12 +179,6 @@
     <t>Data</t>
   </si>
   <si>
-    <t>Printed</t>
-  </si>
-  <si>
-    <t>Enter partial prodct name</t>
-  </si>
-  <si>
     <t>No</t>
   </si>
   <si>
@@ -354,6 +327,72 @@
   </si>
   <si>
     <t>TS_15</t>
+  </si>
+  <si>
+    <t>TC006_DeleteOrder</t>
+  </si>
+  <si>
+    <t>To select a pet and signin while placing the order</t>
+  </si>
+  <si>
+    <t>To delete a already placed order</t>
+  </si>
+  <si>
+    <t>Navigate to My Orders Screen</t>
+  </si>
+  <si>
+    <t>navigateToMyOrdersScreen</t>
+  </si>
+  <si>
+    <t>selectAnOrder</t>
+  </si>
+  <si>
+    <t>Select an Order on My Orders Screen</t>
+  </si>
+  <si>
+    <t>deleteOrder</t>
+  </si>
+  <si>
+    <t>Delete the Order</t>
+  </si>
+  <si>
+    <t>validateOrderIsDeleted</t>
+  </si>
+  <si>
+    <t>Verify that order was deleted successfully</t>
+  </si>
+  <si>
+    <t>TC002_PlaceOrder</t>
+  </si>
+  <si>
+    <t>TC003_CreateAccount</t>
+  </si>
+  <si>
+    <t>To verify that user is able to remove a pet from Cart</t>
+  </si>
+  <si>
+    <t>TC001_RemovePetFromCart</t>
+  </si>
+  <si>
+    <t>Persian</t>
+  </si>
+  <si>
+    <t>Tiger Shark</t>
+  </si>
+  <si>
+    <t>Remove pet from cart</t>
+  </si>
+  <si>
+    <t>removePetFromCart</t>
+  </si>
+  <si>
+    <t>removeAllPetFromCart</t>
+  </si>
+  <si>
+    <t>Remove all pet from cart</t>
+  </si>
+  <si>
+    <t>Your cart is empty.</t>
   </si>
 </sst>
 </file>
@@ -764,7 +803,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -787,105 +826,105 @@
         <v>18</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
     </row>
     <row customFormat="1" r="2" s="1" spans="1:4">
       <c r="A2" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="D2" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="7" t="s">
-        <v>31</v>
+        <v>113</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>21</v>
+        <v>52</v>
       </c>
       <c r="D3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="8" t="s">
-        <v>32</v>
+        <v>114</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>21</v>
+        <v>52</v>
       </c>
       <c r="D4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="7" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>21</v>
+        <v>52</v>
       </c>
       <c r="D5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="8" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>38</v>
+        <v>103</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>21</v>
+        <v>52</v>
       </c>
       <c r="D6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="8" t="s">
-        <v>40</v>
+        <v>102</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>39</v>
+        <v>104</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="D7" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="8" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="D8" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -904,10 +943,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:C4"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -930,18 +969,21 @@
         <v>13</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row customFormat="1" r="2" s="1" spans="1:4">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>71</v>
+      <c r="B2" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D2" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -952,21 +994,77 @@
         <v>74</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="D3" t="s">
-        <v>75</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="D3"/>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
+      </c>
+      <c r="D4" s="3"/>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D6"/>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D7" s="3"/>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="B8" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="B9" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -980,7 +1078,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:D14"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1003,7 +1101,7 @@
         <v>13</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
     </row>
     <row customFormat="1" r="2" s="1" spans="1:4">
@@ -1011,10 +1109,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1022,13 +1120,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="D3" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1036,13 +1134,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>91</v>
-      </c>
       <c r="D4" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1050,10 +1148,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="D5"/>
     </row>
@@ -1062,10 +1160,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="D6" s="3"/>
     </row>
@@ -1074,13 +1172,13 @@
         <v>9</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -1088,10 +1186,10 @@
         <v>10</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -1099,74 +1197,74 @@
         <v>11</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="D13" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1206,7 +1304,7 @@
         <v>13</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
     </row>
     <row customFormat="1" r="2" s="1" spans="1:4">
@@ -1214,10 +1312,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
     </row>
     <row ht="45" r="3" spans="1:4">
@@ -1225,13 +1323,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1239,10 +1337,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>68</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1250,13 +1348,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -1270,7 +1368,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1293,7 +1391,7 @@
         <v>13</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
     </row>
     <row customFormat="1" r="2" s="1" spans="1:4">
@@ -1301,10 +1399,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
     </row>
     <row ht="45" r="3" spans="1:4">
@@ -1312,13 +1410,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1326,10 +1424,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>68</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1337,10 +1435,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -1348,13 +1446,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>91</v>
-      </c>
       <c r="D6" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -1362,10 +1460,10 @@
         <v>9</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="D7"/>
     </row>
@@ -1374,10 +1472,10 @@
         <v>10</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="D8" s="3"/>
     </row>
@@ -1386,99 +1484,99 @@
         <v>11</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="D15" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="1" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1489,10 +1587,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="A2" sqref="A2:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1515,7 +1613,7 @@
         <v>13</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1523,13 +1621,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>91</v>
-      </c>
       <c r="D2" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1537,10 +1635,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="D3"/>
     </row>
@@ -1549,10 +1647,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="D4" s="3"/>
     </row>
@@ -1561,10 +1659,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -1572,13 +1670,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="D6" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -1586,10 +1684,10 @@
         <v>9</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -1597,13 +1695,13 @@
         <v>10</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -1611,49 +1709,61 @@
         <v>11</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="D11" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>69</v>
+        <v>110</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>70</v>
+        <v>109</v>
+      </c>
+      <c r="D12" s="3"/>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1667,24 +1777,22 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="3" width="6.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="3" width="71.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="3" width="29.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="3" width="21.5703125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="3" width="18.5703125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="1" width="20.7109375" collapsed="true"/>
-    <col min="7" max="16384" style="3" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="3" width="5.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="3" width="53.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="3" width="28.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="1" width="70.140625" collapsed="true"/>
+    <col min="5" max="16384" style="3" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="6" spans="1:6">
+    <row customFormat="1" r="1" s="6" spans="1:4">
       <c r="A1" s="4" t="s">
         <v>12</v>
       </c>
@@ -1695,107 +1803,86 @@
         <v>13</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+        <v>51</v>
+      </c>
+    </row>
+    <row customFormat="1" r="2" s="1" spans="1:4">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>60</v>
+      <c r="B2" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>51</v>
+        <v>65</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>64</v>
+      </c>
+      <c r="D3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="B4" s="3" t="s">
+        <v>105</v>
+      </c>
       <c r="C4" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+        <v>106</v>
+      </c>
+      <c r="D4"/>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>52</v>
+        <v>108</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+        <v>107</v>
+      </c>
+      <c r="D5"/>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>53</v>
+        <v>110</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>6</v>
-      </c>
+        <v>109</v>
+      </c>
+      <c r="D6" s="3"/>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="D7" s="3"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink display="test321@yahoo.com" r:id="rId1" ref="F3"/>
+  </hyperlinks>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
@@ -1830,13 +1917,13 @@
         <v>13</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>14</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -1844,19 +1931,19 @@
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1864,16 +1951,16 @@
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1881,16 +1968,16 @@
         <v>2</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1898,19 +1985,19 @@
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1918,13 +2005,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
added test for updating account info, billing and shipping address
</commit_message>
<xml_diff>
--- a/src/test/resources/data/TestDataSheet.xlsx
+++ b/src/test/resources/data/TestDataSheet.xlsx
@@ -4,24 +4,24 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView windowHeight="3855" windowWidth="14820" xWindow="0" yWindow="2520"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="14820" windowHeight="3855" tabRatio="752" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="TestCases" r:id="rId1" sheetId="4"/>
-    <sheet name="TC001_RemovePetFromCart" r:id="rId2" sheetId="3"/>
-    <sheet name="TC002_PlaceOrder" r:id="rId3" sheetId="2"/>
-    <sheet name="TC003_CreateAccount" r:id="rId4" sheetId="5"/>
-    <sheet name="TC004_PlaceOrderWithNewAccount" r:id="rId5" sheetId="6"/>
-    <sheet name="TC005_PlaceOrderAndSignIn" r:id="rId6" sheetId="7"/>
-    <sheet name="TC006_DeleteOrder" r:id="rId7" sheetId="8"/>
-    <sheet name="TC007_CompleteWordSearchTest" r:id="rId8" sheetId="9"/>
+    <sheet name="TestCases" sheetId="4" r:id="rId1"/>
+    <sheet name="TC001_RemovePetFromCart" sheetId="3" r:id="rId2"/>
+    <sheet name="TC002_PlaceOrder" sheetId="2" r:id="rId3"/>
+    <sheet name="TC003_CreateAccount" sheetId="5" r:id="rId4"/>
+    <sheet name="TC004_PlaceOrderWithNewAccount" sheetId="6" r:id="rId5"/>
+    <sheet name="TC005_PlaceOrderAndSignIn" sheetId="7" r:id="rId6"/>
+    <sheet name="TC006_DeleteOrder" sheetId="8" r:id="rId7"/>
+    <sheet name="TC007_UpdateMyAccount" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="130">
   <si>
     <t>TS_01</t>
   </si>
@@ -38,18 +38,6 @@
     <t>TS_05</t>
   </si>
   <si>
-    <t>click</t>
-  </si>
-  <si>
-    <t>xpath</t>
-  </si>
-  <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>enterText</t>
-  </si>
-  <si>
     <t>TS_06</t>
   </si>
   <si>
@@ -65,9 +53,6 @@
     <t>Action Keyword</t>
   </si>
   <si>
-    <t>Element Locator</t>
-  </si>
-  <si>
     <t>Step Description</t>
   </si>
   <si>
@@ -86,9 +71,6 @@
     <t>2</t>
   </si>
   <si>
-    <t>name</t>
-  </si>
-  <si>
     <t>confirmOrder</t>
   </si>
   <si>
@@ -125,63 +107,12 @@
     <t>To verify that user is able to place an order successfully as registered user</t>
   </si>
   <si>
-    <t>TC007_CompleteWordSearchTest</t>
-  </si>
-  <si>
-    <t>To validate search result with complete word search</t>
-  </si>
-  <si>
-    <t>searchBox</t>
-  </si>
-  <si>
-    <t>searchButton</t>
-  </si>
-  <si>
-    <t>searchResultHeading</t>
-  </si>
-  <si>
-    <t>validateSearchResults</t>
-  </si>
-  <si>
-    <t>searchResults</t>
-  </si>
-  <si>
-    <t>validateSearchResultCount</t>
-  </si>
-  <si>
-    <t>searchResultCount</t>
-  </si>
-  <si>
-    <t>Blouse</t>
-  </si>
-  <si>
-    <t>Search for the product</t>
-  </si>
-  <si>
-    <t>Verify that search result is same as the product searched</t>
-  </si>
-  <si>
-    <t>Verify that search result count is same as the product displayed on the screen.</t>
-  </si>
-  <si>
-    <t>Enter complete prodct name</t>
-  </si>
-  <si>
-    <t>validateDataOnScreenContains</t>
-  </si>
-  <si>
     <t>PASS</t>
   </si>
   <si>
-    <t>Object</t>
-  </si>
-  <si>
     <t>Data</t>
   </si>
   <si>
-    <t>No</t>
-  </si>
-  <si>
     <t>Navigate to user Registration screen</t>
   </si>
   <si>
@@ -191,12 +122,6 @@
     <t/>
   </si>
   <si>
-    <t>enterRegisterationDetails</t>
-  </si>
-  <si>
-    <t>Enter Registration details</t>
-  </si>
-  <si>
     <t>Verify Registration is success</t>
   </si>
   <si>
@@ -230,9 +155,6 @@
     <t>clickSaveButton</t>
   </si>
   <si>
-    <t>User|auto123|auto123|John|Doe|auto@gmail.com|9876543210|9010 High Point St|Sierra Street|Houston|Texas|77076|United State|German|Dogs|Yes|Yes</t>
-  </si>
-  <si>
     <t>Iguana</t>
   </si>
   <si>
@@ -299,12 +221,6 @@
     <t>validateOrderDetails</t>
   </si>
   <si>
-    <t>Iguana|2</t>
-  </si>
-  <si>
-    <t>Parrot|1</t>
-  </si>
-  <si>
     <t>Parrot</t>
   </si>
   <si>
@@ -314,27 +230,18 @@
     <t>4</t>
   </si>
   <si>
-    <t>Finch|4</t>
-  </si>
-  <si>
     <t>Login to store with newly created user</t>
   </si>
   <si>
     <t>loginWithNewUser</t>
   </si>
   <si>
-    <t>New|auto123|auto123|John|Doe|auto@gmail.com|9876543210|9010 High Point St|Sierra Street|Houston|Texas|77076|United State|German|Dogs|Yes|Yes</t>
-  </si>
-  <si>
     <t>TS_15</t>
   </si>
   <si>
     <t>TC006_DeleteOrder</t>
   </si>
   <si>
-    <t>To select a pet and signin while placing the order</t>
-  </si>
-  <si>
     <t>To delete a already placed order</t>
   </si>
   <si>
@@ -374,9 +281,6 @@
     <t>TC001_RemovePetFromCart</t>
   </si>
   <si>
-    <t>Persian</t>
-  </si>
-  <si>
     <t>Tiger Shark</t>
   </si>
   <si>
@@ -393,13 +297,126 @@
   </si>
   <si>
     <t>Your cart is empty.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Select a pet </t>
+  </si>
+  <si>
+    <t>Select pet from Category</t>
+  </si>
+  <si>
+    <t>selectPetCategory</t>
+  </si>
+  <si>
+    <t>Cats</t>
+  </si>
+  <si>
+    <t>Select first pet by it ID</t>
+  </si>
+  <si>
+    <t>selectPetByID</t>
+  </si>
+  <si>
+    <t>updatePaymentDetails</t>
+  </si>
+  <si>
+    <t>updateBillingAddress</t>
+  </si>
+  <si>
+    <t>changeShippingAddress</t>
+  </si>
+  <si>
+    <t>updateShippingAddress</t>
+  </si>
+  <si>
+    <t>Update payment details</t>
+  </si>
+  <si>
+    <t>MasterCard|123456789012|12/2024</t>
+  </si>
+  <si>
+    <t>Jane|Doe|901 San Antonio Road|SW 32|Washington DC|LA|93456|United State</t>
+  </si>
+  <si>
+    <t>Update billing address</t>
+  </si>
+  <si>
+    <t>Update shipping address</t>
+  </si>
+  <si>
+    <t>Continue to shipping address</t>
+  </si>
+  <si>
+    <t>Choose to change shipping address</t>
+  </si>
+  <si>
+    <t>TS_16</t>
+  </si>
+  <si>
+    <t>TS_17</t>
+  </si>
+  <si>
+    <t>John|Doe|LA Galaxy|901 San Antonio Road|New York City|New York|78931|United State</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>To select a pet and signin while placing the order and change billing and shipping address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To update account details </t>
+  </si>
+  <si>
+    <t>TC007_UpdateMyAccount</t>
+  </si>
+  <si>
+    <t>enterAccountInformation</t>
+  </si>
+  <si>
+    <t>Update account information</t>
+  </si>
+  <si>
+    <t>Your account has been updated.</t>
+  </si>
+  <si>
+    <t>Verify account update is success</t>
+  </si>
+  <si>
+    <t>Save account details</t>
+  </si>
+  <si>
+    <t>John|Doe|auto@gmail.com|9876543210|9010 High Point St|Sierra Street|Houston|Texas|77076|United State|German|Dogs|No|Yes</t>
+  </si>
+  <si>
+    <t>User|auto123|auto123</t>
+  </si>
+  <si>
+    <t>Enter account information</t>
+  </si>
+  <si>
+    <t>Enter User Information</t>
+  </si>
+  <si>
+    <t>enterUserInformation</t>
+  </si>
+  <si>
+    <t>Navigate to user Account screen</t>
+  </si>
+  <si>
+    <t>navigateToMyAccountScreen</t>
+  </si>
+  <si>
+    <t>Jane|Doe|test321@gmail.com|9876543210|9010 High Point St|Sierra Street|Houston|Texas|77076|United State|German|Dogs|No|Yes</t>
+  </si>
+  <si>
+    <t>John|Doe|auto@gmail.com|9876543210|9010 High Point St|Sierra Street|Houston|Texas|77076|United State|German|Dogs|Yes|Yes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -474,44 +491,50 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
+  <cellXfs count="12">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="2" fontId="1" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="2" fontId="1" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="2" fontId="1" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="1"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
@@ -520,10 +543,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -679,7 +702,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -688,13 +711,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -704,7 +727,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -713,7 +736,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -722,7 +745,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -732,12 +755,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
+            <a:lightRig rig="threePt" dir="t">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT h="25400" w="63500"/>
+            <a:bevelT w="63500" h="25400"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -768,7 +791,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -787,7 +810,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -800,176 +823,176 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="3" width="37.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="3" width="67.5703125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="3" width="10.140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="3" width="15.85546875" collapsed="true"/>
-    <col min="5" max="16384" style="3" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="37.140625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="81.85546875" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.140625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15.85546875" style="3" customWidth="1" collapsed="1"/>
+    <col min="5" max="16384" width="9.140625" style="3" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="2" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row customFormat="1" r="2" s="1" spans="1:4">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" s="1" customFormat="1">
       <c r="A2" s="7" t="s">
-        <v>116</v>
+        <v>85</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>115</v>
+        <v>84</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="7" t="s">
-        <v>113</v>
+        <v>82</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>52</v>
+        <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>55</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="8" t="s">
-        <v>114</v>
+        <v>83</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>52</v>
+        <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>55</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="7" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>52</v>
+        <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>55</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" t="s">
         <v>32</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D6" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="8" t="s">
-        <v>102</v>
+        <v>72</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>104</v>
+        <v>73</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>52</v>
+        <v>14</v>
       </c>
       <c r="D7" t="s">
-        <v>55</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="8" t="s">
-        <v>34</v>
+        <v>115</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>35</v>
+        <v>114</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>52</v>
+        <v>14</v>
       </c>
       <c r="D8" t="s">
-        <v>55</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink display="TC001_LoginTest" location="TC001_LoginTest!A1" ref="A2"/>
-    <hyperlink display="TC002_PlaceOrderTest" location="TC002_PlaceOrderTest!A1" ref="A3"/>
-    <hyperlink display="TC003_CreateAccountTest" location="TC003_CreateAccountTest!A1" ref="A4"/>
-    <hyperlink display="TC004_PlaceOrderWithNewAccount" location="TC004_PlaceOrderWithNewAccount!A1" ref="A5"/>
-    <hyperlink display="TC005_PlaceOrderAndSignIn" location="TC005_PlaceOrderAndSignIn!A1" ref="A6"/>
-    <hyperlink display="TC006_PartialWordSearchTest" location="TC006_PartialWordSearchTest!A1" ref="A7"/>
-    <hyperlink display="TC007_CompleteWordSearchTest" location="TC007_CompleteWordSearchTest!A1" ref="A8"/>
+    <hyperlink ref="A2" location="TC001_LoginTest!A1" display="TC001_LoginTest"/>
+    <hyperlink ref="A3" location="TC002_PlaceOrderTest!A1" display="TC002_PlaceOrderTest"/>
+    <hyperlink ref="A4" location="TC003_CreateAccountTest!A1" display="TC003_CreateAccountTest"/>
+    <hyperlink ref="A5" location="TC004_PlaceOrderWithNewAccount!A1" display="TC004_PlaceOrderWithNewAccount"/>
+    <hyperlink ref="A6" location="TC005_PlaceOrderAndSignIn!A1" display="TC005_PlaceOrderAndSignIn"/>
+    <hyperlink ref="A7" location="TC006_PartialWordSearchTest!A1" display="TC006_PartialWordSearchTest"/>
+    <hyperlink ref="A8" location="TC007_CompleteWordSearchTest!A1" display="TC007_CompleteWordSearchTest"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="3" width="5.7109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="3" width="53.5703125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="3" width="28.7109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="1" width="70.140625" collapsed="true"/>
-    <col min="5" max="16384" style="3" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="5.7109375" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="53.5703125" style="3" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="28.7109375" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="70.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="16384" width="9.140625" style="3" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="6" spans="1:4">
+    <row r="1" spans="1:4" s="6" customFormat="1">
       <c r="A1" s="4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>51</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -977,13 +1000,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>73</v>
+        <v>47</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>82</v>
+        <v>56</v>
       </c>
       <c r="D2" t="s">
-        <v>117</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -991,10 +1014,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>74</v>
+        <v>48</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>81</v>
+        <v>55</v>
       </c>
       <c r="D3"/>
     </row>
@@ -1003,116 +1026,134 @@
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>75</v>
+        <v>49</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>71</v>
+        <v>45</v>
       </c>
       <c r="D4" s="3"/>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>73</v>
+        <v>93</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>82</v>
+        <v>94</v>
       </c>
       <c r="D5" t="s">
-        <v>118</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>74</v>
+        <v>92</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>81</v>
+        <v>55</v>
       </c>
       <c r="D6"/>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="D7" s="3"/>
+        <v>97</v>
+      </c>
+      <c r="D7"/>
     </row>
     <row r="8" spans="1:4">
+      <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="B8" s="3" t="s">
-        <v>119</v>
+        <v>49</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>120</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="D8" s="3"/>
     </row>
     <row r="9" spans="1:4">
+      <c r="A9" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="B9" s="3" t="s">
-        <v>122</v>
+        <v>87</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>123</v>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="300" orientation="portrait" r:id="rId1" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="A2" sqref="A2:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="3" width="5.7109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="3" width="53.5703125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="3" width="28.7109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="1" width="70.140625" collapsed="true"/>
-    <col min="5" max="16384" style="3" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="5.7109375" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="53.5703125" style="3" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="28.7109375" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="70.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="16384" width="9.140625" style="3" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="6" spans="1:4">
+    <row r="1" spans="1:4" s="6" customFormat="1">
       <c r="A1" s="4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row customFormat="1" r="2" s="1" spans="1:4">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" s="1" customFormat="1">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>63</v>
+        <v>38</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>62</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1120,13 +1161,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>64</v>
+        <v>39</v>
       </c>
       <c r="D3" t="s">
-        <v>66</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1134,13 +1175,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>73</v>
+        <v>47</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>82</v>
+        <v>56</v>
       </c>
       <c r="D4" t="s">
-        <v>70</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1148,10 +1189,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>74</v>
+        <v>48</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>81</v>
+        <v>55</v>
       </c>
       <c r="D5"/>
     </row>
@@ -1160,187 +1201,190 @@
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>75</v>
+        <v>49</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>71</v>
+        <v>45</v>
       </c>
       <c r="D6" s="3"/>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>78</v>
+        <v>52</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>79</v>
+        <v>53</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>76</v>
+        <v>50</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>77</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>84</v>
+        <v>58</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>83</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>85</v>
+        <v>59</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>89</v>
+        <v>63</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>88</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>86</v>
+        <v>60</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>87</v>
+        <v>61</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>72</v>
+        <v>46</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>80</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>90</v>
+        <v>64</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="D13" t="s">
-        <v>92</v>
+        <v>65</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>60</v>
+        <v>35</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>61</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink display="test321@yahoo.com" r:id="rId1" ref="F3"/>
+    <hyperlink ref="F3" r:id="rId1" display="test321@yahoo.com"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="300" orientation="portrait" r:id="rId2" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="3" width="5.7109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="3" width="53.5703125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="3" width="28.7109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="1" width="67.5703125" collapsed="true"/>
-    <col min="5" max="16384" style="3" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="5.7109375" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="53.5703125" style="3" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="28.7109375" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="67.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="16384" width="9.140625" style="3" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="6" spans="1:4">
+    <row r="1" spans="1:4" s="6" customFormat="1">
       <c r="A1" s="4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row customFormat="1" r="2" s="1" spans="1:4">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" s="1" customFormat="1">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>53</v>
+        <v>30</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row ht="45" r="3" spans="1:4">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>57</v>
+        <v>124</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>56</v>
+        <v>125</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="30">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>59</v>
+        <v>123</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>68</v>
+        <v>116</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1348,86 +1392,100 @@
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>58</v>
+        <v>34</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>67</v>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="300" orientation="portrait" r:id="rId1" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A4" sqref="A4:A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="3" width="5.7109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="3" width="53.5703125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="3" width="28.7109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="1" width="67.5703125" collapsed="true"/>
-    <col min="5" max="16384" style="3" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="5.7109375" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="53.5703125" style="3" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="28.7109375" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="67.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="16384" width="9.140625" style="3" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="6" spans="1:4">
+    <row r="1" spans="1:4" s="6" customFormat="1">
       <c r="A1" s="4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row customFormat="1" r="2" s="1" spans="1:4">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" s="1" customFormat="1">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>53</v>
+        <v>30</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row ht="45" r="3" spans="1:4">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>57</v>
+        <v>124</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>56</v>
+        <v>125</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="30">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>59</v>
+        <v>123</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>68</v>
+        <v>116</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1435,10 +1493,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>98</v>
+        <v>34</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>99</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -1446,174 +1504,185 @@
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="D6" t="s">
-        <v>95</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>74</v>
+        <v>47</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="D7"/>
+        <v>56</v>
+      </c>
+      <c r="D7" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>75</v>
+        <v>48</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="D8" s="3"/>
+        <v>55</v>
+      </c>
+      <c r="D8"/>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>78</v>
+        <v>49</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>96</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="D9" s="3"/>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>77</v>
+        <v>52</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>84</v>
+        <v>50</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>83</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>88</v>
+        <v>58</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>86</v>
+        <v>59</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>22</v>
+        <v>63</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>87</v>
+        <v>60</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>80</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>90</v>
+        <v>61</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="D15" t="s">
-        <v>97</v>
+        <v>46</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="1" t="s">
-        <v>101</v>
+        <v>71</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>61</v>
+        <v>65</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="300" orientation="portrait" r:id="rId1" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD4"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="3" width="5.7109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="3" width="53.5703125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="3" width="28.7109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="1" width="70.140625" collapsed="true"/>
-    <col min="5" max="16384" style="3" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="5.7109375" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="53.5703125" style="3" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="28.7109375" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="82.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="16384" width="9.140625" style="3" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="6" spans="1:4">
+    <row r="1" spans="1:4" s="6" customFormat="1">
       <c r="A1" s="4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>51</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1621,13 +1690,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>73</v>
+        <v>47</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>82</v>
+        <v>56</v>
       </c>
       <c r="D2" t="s">
-        <v>94</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1635,10 +1704,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>74</v>
+        <v>48</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>81</v>
+        <v>55</v>
       </c>
       <c r="D3"/>
     </row>
@@ -1647,10 +1716,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>75</v>
+        <v>49</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>71</v>
+        <v>45</v>
       </c>
       <c r="D4" s="3"/>
     </row>
@@ -1659,10 +1728,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>76</v>
+        <v>50</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>77</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -1670,114 +1739,178 @@
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>64</v>
+        <v>39</v>
       </c>
       <c r="D6" t="s">
-        <v>66</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>83</v>
+        <v>102</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>85</v>
+        <v>105</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>88</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>86</v>
+        <v>108</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>22</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>80</v>
+        <v>107</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>90</v>
+        <v>106</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="D11" t="s">
-        <v>93</v>
+        <v>101</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="D12" s="3"/>
+        <v>58</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B13" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C14" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>61</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D17" s="3"/>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink display="test321@yahoo.com" r:id="rId1" ref="F6"/>
+    <hyperlink ref="F6" r:id="rId1" display="test321@yahoo.com"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="300" orientation="portrait" r:id="rId2" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6:XFD6"/>
@@ -1785,36 +1918,36 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="3" width="5.7109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="3" width="53.5703125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="3" width="28.7109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="1" width="70.140625" collapsed="true"/>
-    <col min="5" max="16384" style="3" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="5.7109375" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="53.5703125" style="3" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="28.7109375" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="70.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="16384" width="9.140625" style="3" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="6" spans="1:4">
+    <row r="1" spans="1:4" s="6" customFormat="1">
       <c r="A1" s="4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row customFormat="1" r="2" s="1" spans="1:4">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" s="1" customFormat="1">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>63</v>
+        <v>38</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>62</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1822,13 +1955,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>64</v>
+        <v>39</v>
       </c>
       <c r="D3" t="s">
-        <v>66</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1836,10 +1969,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>105</v>
+        <v>74</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>106</v>
+        <v>75</v>
       </c>
       <c r="D4"/>
     </row>
@@ -1848,10 +1981,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>108</v>
+        <v>77</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>107</v>
+        <v>76</v>
       </c>
       <c r="D5"/>
     </row>
@@ -1860,164 +1993,143 @@
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>110</v>
+        <v>79</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>109</v>
+        <v>78</v>
       </c>
       <c r="D6" s="3"/>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>112</v>
+        <v>81</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>111</v>
+        <v>80</v>
       </c>
       <c r="D7" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink display="test321@yahoo.com" r:id="rId1" ref="F3"/>
+    <hyperlink ref="F3" r:id="rId1" display="test321@yahoo.com"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="3" width="6.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="3" width="71.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="3" width="29.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="3" width="21.5703125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="3" width="18.5703125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="1" width="20.7109375" collapsed="true"/>
-    <col min="7" max="16384" style="3" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="5.7109375" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="53.5703125" style="3" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="28.7109375" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="67.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="16384" width="9.140625" style="3" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="6" spans="1:6">
+    <row r="1" spans="1:4" s="6" customFormat="1">
       <c r="A1" s="4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" s="1" customFormat="1">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>47</v>
+      <c r="B2" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>39</v>
+      </c>
+      <c r="D3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="1" customFormat="1">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="B4" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="30">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>45</v>
+        <v>117</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+        <v>116</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>6</v>
+      <c r="D7" s="1" t="s">
+        <v>118</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <hyperlinks>
+    <hyperlink ref="F3" r:id="rId1" display="test321@yahoo.com"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>